<commit_message>
adjusted family names in rules, to conveniently compare with old grassius
</commit_message>
<xml_diff>
--- a/inputs/private_inputs/Current_TF_family_rules.xlsx
+++ b/inputs/private_inputs/Current_TF_family_rules.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="469">
   <si>
     <t xml:space="preserve">familyname(orig)</t>
   </si>
@@ -179,9 +179,6 @@
     <t xml:space="preserve">B3</t>
   </si>
   <si>
-    <t xml:space="preserve">ABI3VP1</t>
-  </si>
-  <si>
     <t xml:space="preserve">B3:PF02362</t>
   </si>
   <si>
@@ -545,7 +542,7 @@
     <t xml:space="preserve">FAR1</t>
   </si>
   <si>
-    <t xml:space="preserve">FAR</t>
+    <t xml:space="preserve">FAR1-like</t>
   </si>
   <si>
     <t xml:space="preserve">FAR1:PF03101</t>
@@ -698,6 +695,9 @@
     <t xml:space="preserve">LFY</t>
   </si>
   <si>
+    <t xml:space="preserve">FLO/LFY</t>
+  </si>
+  <si>
     <t xml:space="preserve">FLO_LFY (PF01698)</t>
   </si>
   <si>
@@ -797,9 +797,6 @@
     <t xml:space="preserve">OFP</t>
   </si>
   <si>
-    <t xml:space="preserve">Ovate</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ovate (PF04844)</t>
   </si>
   <si>
@@ -827,6 +824,9 @@
     <t xml:space="preserve">Rcd1L</t>
   </si>
   <si>
+    <t xml:space="preserve">Rcd1-like</t>
+  </si>
+  <si>
     <t xml:space="preserve">RCD1(PF04078)</t>
   </si>
   <si>
@@ -948,9 +948,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIFFY</t>
   </si>
   <si>
     <t xml:space="preserve">tify (PF06200)</t>
@@ -1440,7 +1437,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1503,6 +1500,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -1557,7 +1560,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1610,7 +1613,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1618,7 +1625,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1641,10 +1648,10 @@
   </sheetPr>
   <dimension ref="A1:AH89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2084,28 +2091,28 @@
         <v>51</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="K8" s="5" t="n">
         <v>12897250</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="9"/>
@@ -2132,28 +2139,28 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="5"/>
@@ -2161,7 +2168,7 @@
         <v>11906833</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="9"/>
@@ -2188,28 +2195,28 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="5"/>
@@ -2217,10 +2224,10 @@
         <v>15680330</v>
       </c>
       <c r="L10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -2246,28 +2253,28 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="5"/>
@@ -2275,7 +2282,7 @@
         <v>11018156</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="9"/>
@@ -2302,40 +2309,40 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="I12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="K12" s="5" t="n">
         <v>15111712</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="9"/>
@@ -2362,40 +2369,40 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="K13" s="5" t="n">
         <v>15084732</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="9"/>
@@ -2422,28 +2429,28 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="5"/>
@@ -2451,7 +2458,7 @@
         <v>10679447</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="9"/>
@@ -2478,28 +2485,28 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="5"/>
@@ -2507,7 +2514,7 @@
         <v>21803862</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="9"/>
@@ -2534,28 +2541,28 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="5"/>
@@ -2563,7 +2570,7 @@
         <v>9501112</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="9"/>
@@ -2590,40 +2597,40 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="I17" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="J17" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="K17" s="5" t="n">
         <v>19270186</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="9"/>
@@ -2650,34 +2657,34 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="I18" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -2706,28 +2713,28 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="5"/>
@@ -2735,7 +2742,7 @@
         <v>9612081</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="9"/>
@@ -2762,38 +2769,38 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G20" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="I20" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="J20" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="K20" s="5" t="n">
         <v>9612081</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="9"/>
@@ -2820,40 +2827,40 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="I21" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="J21" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="K21" s="10" t="n">
         <v>9612081</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
@@ -2880,40 +2887,40 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="H22" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="I22" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="K22" s="5" t="n">
         <v>9612081</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="9"/>
@@ -2940,40 +2947,40 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="I23" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="J23" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="K23" s="5" t="n">
         <v>25730064</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="9"/>
@@ -3000,28 +3007,28 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="G24" s="5" t="s">
+      <c r="H24" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="5"/>
@@ -3029,7 +3036,7 @@
         <v>1622933</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="9"/>
@@ -3056,28 +3063,28 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>155</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="5"/>
@@ -3085,10 +3092,10 @@
         <v>16666616</v>
       </c>
       <c r="L25" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="M25" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
@@ -3114,28 +3121,28 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="5"/>
@@ -3143,7 +3150,7 @@
         <v>15308755</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M26" s="5"/>
       <c r="N26" s="9"/>
@@ -3170,28 +3177,28 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G27" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>165</v>
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="5"/>
@@ -3199,7 +3206,7 @@
         <v>11359609</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="9"/>
@@ -3226,28 +3233,28 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>169</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="5"/>
@@ -3255,7 +3262,7 @@
         <v>16407444</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M28" s="5"/>
       <c r="N28" s="9"/>
@@ -3282,28 +3289,28 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>172</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="5"/>
@@ -3311,7 +3318,7 @@
         <v>18033885</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M29" s="5"/>
       <c r="N29" s="9"/>
@@ -3338,40 +3345,40 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="I30" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="J30" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="K30" s="5" t="n">
         <v>21515819</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M30" s="5"/>
       <c r="N30" s="9"/>
@@ -3398,43 +3405,43 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="G31" s="5" t="s">
+      <c r="H31" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="I31" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="J31" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="K31" s="5" t="n">
         <v>22745430</v>
       </c>
       <c r="L31" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
@@ -3460,28 +3467,28 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G32" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>197</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>198</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="5"/>
@@ -3489,7 +3496,7 @@
         <v>18162594</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M32" s="5"/>
       <c r="N32" s="9"/>
@@ -3516,28 +3523,28 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="8" t="s">
         <v>201</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>202</v>
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="5"/>
@@ -3545,7 +3552,7 @@
         <v>19820314</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M33" s="5"/>
       <c r="N33" s="9"/>
@@ -3572,28 +3579,28 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="I34" s="8"/>
       <c r="J34" s="5"/>
@@ -3601,7 +3608,7 @@
         <v>25620770</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M34" s="5"/>
       <c r="N34" s="9"/>
@@ -3628,28 +3635,28 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="F35" s="5" t="s">
+      <c r="G35" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="8" t="s">
         <v>212</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>213</v>
       </c>
       <c r="I35" s="8"/>
       <c r="J35" s="5"/>
@@ -3657,7 +3664,7 @@
         <v>19734295</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M35" s="5"/>
       <c r="N35" s="9"/>
@@ -3684,28 +3691,28 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G36" s="6" t="s">
+      <c r="H36" s="7" t="s">
         <v>216</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="5"/>
@@ -3713,7 +3720,7 @@
         <v>9722564</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M36" s="5"/>
       <c r="N36" s="9"/>
@@ -3740,28 +3747,28 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="G37" s="6" t="s">
+      <c r="H37" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="5"/>
@@ -3769,7 +3776,7 @@
         <v>26904076</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M37" s="5"/>
       <c r="N37" s="9"/>
@@ -3796,22 +3803,22 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>224</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>225</v>
@@ -4030,7 +4037,7 @@
         <v>246</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>246</v>
@@ -4146,16 +4153,16 @@
         <v>257</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>257</v>
       </c>
       <c r="G44" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="H44" s="8" t="s">
         <v>259</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>260</v>
       </c>
       <c r="I44" s="8"/>
       <c r="J44" s="5"/>
@@ -4163,7 +4170,7 @@
         <v>24987011</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="9"/>
@@ -4190,28 +4197,28 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="G45" s="5" t="s">
+      <c r="H45" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>264</v>
       </c>
       <c r="I45" s="8"/>
       <c r="J45" s="5"/>
@@ -4219,7 +4226,7 @@
         <v>12183381</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M45" s="5"/>
       <c r="N45" s="9"/>
@@ -4246,22 +4253,22 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>268</v>
@@ -4304,26 +4311,26 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>272</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>273</v>
@@ -4709,32 +4716,32 @@
       <c r="D54" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="E54" s="5" t="s">
-        <v>309</v>
+      <c r="E54" s="13" t="s">
+        <v>307</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>308</v>
       </c>
       <c r="G54" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="H54" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="H54" s="8" t="s">
+      <c r="I54" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J54" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="I54" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>312</v>
       </c>
       <c r="K54" s="5" t="n">
         <v>10946105</v>
       </c>
       <c r="L54" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="M54" s="5" t="s">
         <v>313</v>
-      </c>
-      <c r="M54" s="5" t="s">
-        <v>314</v>
       </c>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
@@ -4760,28 +4767,28 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>315</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>316</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="E55" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="G55" s="5" t="s">
+      <c r="H55" s="8" t="s">
         <v>318</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>319</v>
       </c>
       <c r="I55" s="8"/>
       <c r="J55" s="5"/>
@@ -4789,7 +4796,7 @@
         <v>27310029</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M55" s="5"/>
       <c r="N55" s="9"/>
@@ -4816,28 +4823,28 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="G56" s="5" t="s">
+      <c r="H56" s="8" t="s">
         <v>322</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>323</v>
       </c>
       <c r="I56" s="8"/>
       <c r="J56" s="5"/>
@@ -4845,10 +4852,10 @@
         <v>22236699</v>
       </c>
       <c r="L56" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="M56" s="5" t="s">
         <v>324</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>325</v>
       </c>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
@@ -4874,28 +4881,28 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="G57" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="E57" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="G57" s="5" t="s">
+      <c r="H57" s="8" t="s">
         <v>327</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>328</v>
       </c>
       <c r="I57" s="8"/>
       <c r="J57" s="5"/>
@@ -4903,7 +4910,7 @@
         <v>15064372</v>
       </c>
       <c r="L57" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M57" s="5"/>
       <c r="N57" s="9"/>
@@ -4930,28 +4937,28 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D58" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="G58" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="E58" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="G58" s="5" t="s">
+      <c r="H58" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>333</v>
       </c>
       <c r="I58" s="8"/>
       <c r="J58" s="5"/>
@@ -4959,7 +4966,7 @@
         <v>15295067</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M58" s="5"/>
       <c r="N58" s="9"/>
@@ -4986,28 +4993,28 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="E59" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="G59" s="5" t="s">
+      <c r="H59" s="8" t="s">
         <v>336</v>
-      </c>
-      <c r="H59" s="8" t="s">
-        <v>337</v>
       </c>
       <c r="I59" s="8"/>
       <c r="J59" s="5"/>
@@ -5015,10 +5022,10 @@
         <v>15708347</v>
       </c>
       <c r="L59" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="M59" s="5" t="s">
         <v>338</v>
-      </c>
-      <c r="M59" s="5" t="s">
-        <v>339</v>
       </c>
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
@@ -5044,28 +5051,28 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>340</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>341</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G60" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="H60" s="8" t="s">
         <v>342</v>
-      </c>
-      <c r="H60" s="8" t="s">
-        <v>343</v>
       </c>
       <c r="I60" s="8"/>
       <c r="J60" s="5"/>
@@ -5073,7 +5080,7 @@
         <v>20304701</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M60" s="5"/>
       <c r="N60" s="9"/>
@@ -5100,26 +5107,26 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="H61" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="H61" s="8" t="s">
-        <v>347</v>
       </c>
       <c r="I61" s="8"/>
       <c r="J61" s="5"/>
@@ -5127,10 +5134,10 @@
         <v>11289511</v>
       </c>
       <c r="L61" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="M61" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="M61" s="5" t="s">
-        <v>349</v>
       </c>
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
@@ -5156,26 +5163,26 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>350</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>351</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="H62" s="8" t="s">
         <v>353</v>
-      </c>
-      <c r="H62" s="8" t="s">
-        <v>354</v>
       </c>
       <c r="I62" s="8"/>
       <c r="J62" s="5"/>
@@ -5183,10 +5190,10 @@
         <v>17499004</v>
       </c>
       <c r="L62" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="M62" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="M62" s="5" t="s">
-        <v>356</v>
       </c>
       <c r="N62" s="9"/>
       <c r="O62" s="9"/>
@@ -5212,25 +5219,25 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="G63" s="1" t="s">
+      <c r="H63" s="8" t="s">
         <v>359</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>360</v>
       </c>
       <c r="I63" s="8"/>
       <c r="J63" s="9"/>
@@ -5261,117 +5268,117 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="G64" s="1" t="s">
+      <c r="H64" s="8" t="s">
         <v>362</v>
-      </c>
-      <c r="H64" s="8" t="s">
-        <v>363</v>
       </c>
       <c r="I64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="G65" s="1" t="s">
+      <c r="H65" s="8" t="s">
         <v>365</v>
-      </c>
-      <c r="H65" s="8" t="s">
-        <v>366</v>
       </c>
       <c r="I65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="G66" s="1" t="s">
+      <c r="H66" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="H66" s="8" t="s">
+      <c r="I66" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="I66" s="8" t="s">
+      <c r="J66" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="G67" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="G67" s="10" t="s">
+      <c r="H67" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="H67" s="7" t="s">
+      <c r="I67" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I67" s="7" t="s">
+      <c r="J67" s="10" t="s">
         <v>376</v>
-      </c>
-      <c r="J67" s="10" t="s">
-        <v>377</v>
       </c>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
@@ -5400,33 +5407,33 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G68" s="10" t="s">
         <v>378</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="G68" s="10" t="s">
+      <c r="H68" s="7" t="s">
         <v>379</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>380</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J68" s="13" t="s">
+      <c r="J68" s="14" t="s">
         <v>46</v>
       </c>
       <c r="K68" s="9"/>
@@ -5456,31 +5463,31 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D69" s="1" t="s">
+      <c r="E69" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G69" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="G69" s="1" t="s">
+      <c r="H69" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="H69" s="8" t="s">
-        <v>385</v>
-      </c>
       <c r="I69" s="8"/>
-      <c r="J69" s="13"/>
+      <c r="J69" s="14"/>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
@@ -5508,31 +5515,31 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G70" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="G70" s="1" t="s">
+      <c r="H70" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="H70" s="8" t="s">
-        <v>389</v>
-      </c>
       <c r="I70" s="8"/>
-      <c r="J70" s="13"/>
+      <c r="J70" s="14"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
@@ -5560,31 +5567,31 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="G71" s="1" t="s">
+      <c r="H71" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="H71" s="8" t="s">
-        <v>392</v>
-      </c>
       <c r="I71" s="8"/>
-      <c r="J71" s="13"/>
+      <c r="J71" s="14"/>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
@@ -5612,31 +5619,31 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="G72" s="1" t="s">
+      <c r="H72" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="H72" s="8" t="s">
-        <v>396</v>
-      </c>
       <c r="I72" s="8"/>
-      <c r="J72" s="13"/>
+      <c r="J72" s="14"/>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
@@ -5664,31 +5671,31 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="C73" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D73" s="1" t="s">
+      <c r="E73" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G73" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G73" s="1" t="s">
+      <c r="H73" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="H73" s="8" t="s">
-        <v>401</v>
-      </c>
       <c r="I73" s="8"/>
-      <c r="J73" s="13"/>
+      <c r="J73" s="14"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
@@ -5716,31 +5723,31 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="G74" s="1" t="s">
+      <c r="H74" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="H74" s="8" t="s">
-        <v>405</v>
-      </c>
       <c r="I74" s="8"/>
-      <c r="J74" s="13"/>
+      <c r="J74" s="14"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
@@ -5768,34 +5775,34 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="G75" s="1" t="s">
+      <c r="H75" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="H75" s="8" t="s">
+      <c r="I75" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="I75" s="8" t="s">
+      <c r="J75" s="14" t="s">
         <v>409</v>
-      </c>
-      <c r="J75" s="13" t="s">
-        <v>410</v>
       </c>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
@@ -5824,31 +5831,31 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G76" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="G76" s="10" t="s">
+      <c r="H76" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="H76" s="7" t="s">
-        <v>414</v>
-      </c>
       <c r="I76" s="7"/>
-      <c r="J76" s="13"/>
+      <c r="J76" s="14"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
@@ -5876,34 +5883,34 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C77" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G77" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="G77" s="10" t="s">
+      <c r="H77" s="7" t="s">
         <v>417</v>
-      </c>
-      <c r="H77" s="7" t="s">
-        <v>418</v>
       </c>
       <c r="I77" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="J77" s="13" t="s">
-        <v>419</v>
+      <c r="J77" s="14" t="s">
+        <v>418</v>
       </c>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
@@ -5932,34 +5939,34 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="G78" s="1" t="s">
+      <c r="H78" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="H78" s="8" t="s">
+      <c r="I78" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J78" s="14" t="s">
         <v>422</v>
-      </c>
-      <c r="I78" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="J78" s="13" t="s">
-        <v>423</v>
       </c>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
@@ -5988,31 +5995,31 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="G79" s="1" t="s">
+      <c r="H79" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="H79" s="8" t="s">
-        <v>427</v>
-      </c>
       <c r="I79" s="8"/>
-      <c r="J79" s="13"/>
+      <c r="J79" s="14"/>
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
@@ -6040,34 +6047,34 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G80" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="G80" s="10" t="s">
+      <c r="H80" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="H80" s="7" t="s">
+      <c r="I80" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="I80" s="7" t="s">
+      <c r="J80" s="14" t="s">
         <v>432</v>
-      </c>
-      <c r="J80" s="13" t="s">
-        <v>433</v>
       </c>
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
@@ -6096,31 +6103,31 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G81" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="G81" s="1" t="s">
+      <c r="H81" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="H81" s="8" t="s">
-        <v>436</v>
-      </c>
       <c r="I81" s="8"/>
-      <c r="J81" s="13"/>
+      <c r="J81" s="14"/>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
@@ -6148,34 +6155,34 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="G82" s="1" t="s">
+      <c r="H82" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="H82" s="8" t="s">
+      <c r="I82" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="I82" s="8" t="s">
+      <c r="J82" s="14" t="s">
         <v>440</v>
-      </c>
-      <c r="J82" s="13" t="s">
-        <v>441</v>
       </c>
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
@@ -6204,34 +6211,34 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="G83" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="G83" s="10" t="s">
+      <c r="H83" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="I83" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="H83" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="I83" s="7" t="s">
+      <c r="J83" s="14" t="s">
         <v>444</v>
-      </c>
-      <c r="J83" s="13" t="s">
-        <v>445</v>
       </c>
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
@@ -6260,34 +6267,34 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="G84" s="1" t="s">
+      <c r="H84" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="H84" s="8" t="s">
+      <c r="I84" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="J84" s="14" t="s">
         <v>449</v>
-      </c>
-      <c r="I84" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="J84" s="13" t="s">
-        <v>450</v>
       </c>
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
@@ -6316,34 +6323,34 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="C85" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G85" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>448</v>
-      </c>
       <c r="H85" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="J85" s="13" t="s">
-        <v>450</v>
+        <v>369</v>
+      </c>
+      <c r="J85" s="14" t="s">
+        <v>449</v>
       </c>
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
@@ -6372,31 +6379,31 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="G86" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="G86" s="10" t="s">
+      <c r="H86" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="H86" s="7" t="s">
-        <v>454</v>
-      </c>
       <c r="I86" s="7"/>
-      <c r="J86" s="13"/>
+      <c r="J86" s="14"/>
       <c r="K86" s="9"/>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
@@ -6424,31 +6431,31 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="G87" s="1" t="s">
+      <c r="H87" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="H87" s="8" t="s">
-        <v>457</v>
-      </c>
       <c r="I87" s="8"/>
-      <c r="J87" s="13"/>
+      <c r="J87" s="14"/>
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
       <c r="M87" s="9"/>
@@ -6476,34 +6483,34 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="G88" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="G88" s="10" t="s">
+      <c r="H88" s="8" t="s">
         <v>459</v>
       </c>
-      <c r="H88" s="8" t="s">
+      <c r="I88" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="I88" s="7" t="s">
+      <c r="J88" s="15" t="s">
         <v>461</v>
-      </c>
-      <c r="J88" s="14" t="s">
-        <v>462</v>
       </c>
       <c r="K88" s="9"/>
       <c r="L88" s="9"/>
@@ -6532,34 +6539,34 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>463</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="F89" s="1" t="s">
+      <c r="G89" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="G89" s="1" t="s">
+      <c r="H89" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="H89" s="8" t="s">
+      <c r="I89" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="I89" s="8" t="s">
+      <c r="J89" s="14" t="s">
         <v>467</v>
-      </c>
-      <c r="J89" s="13" t="s">
-        <v>468</v>
       </c>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
@@ -6614,43 +6621,43 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
-        <v>215</v>
+      <c r="A1" s="16" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>317</v>
+      <c r="A2" s="16" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>425</v>
+      <c r="A3" s="16" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>326</v>
+      <c r="A4" s="16" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>186</v>
+      <c r="A5" s="16" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>135</v>
+      <c r="A6" s="16" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>143</v>
+      <c r="A7" s="16" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>469</v>
+      <c r="A8" s="16" t="s">
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleanup, added orphans family, added workaround for iTAK issue with MYB-related family
</commit_message>
<xml_diff>
--- a/inputs/private_inputs/Current_TF_family_rules.xlsx
+++ b/inputs/private_inputs/Current_TF_family_rules.xlsx
@@ -734,6 +734,30 @@
     <t xml:space="preserve">PF00319#1:PF01486#1</t>
   </si>
   <si>
+    <t xml:space="preserve">MYB-related</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYB_related</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myb_DNA-binding (PF00249)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF00249#1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF04433#1:PF01388#1:PF00072#1:PF00176#1:G2-like#1:Trihelix#1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWIRM (PF04433); ARID (PF01388); Response_reg (PF000072); SNF2_N (PF00176); G2-like; Trihelix;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A novel leaf-specific myb-related protein with a single binding repeat.Kirik V1, Bäumlein H</t>
+  </si>
+  <si>
     <t xml:space="preserve">MYB</t>
   </si>
   <si>
@@ -753,30 +777,6 @@
   </si>
   <si>
     <t xml:space="preserve">GRASSIUS  rules add aonther possible domaing: Myb_DNA-binding (&gt; 1) or Myb_DNA- bind_6 binding (&gt;1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MYB-related</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MYBR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MYB_related</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myb_DNA-binding (PF00249)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PF00249#1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PF04433#1:PF01388#1:PF00072#1:PF00176#1:G2-like#1:Trihelix#1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SWIRM (PF04433); ARID (PF01388); Response_reg (PF000072); SNF2_N (PF00176); G2-like; Trihelix;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A novel leaf-specific myb-related protein with a single binding repeat.Kirik V1, Bäumlein H</t>
   </si>
   <si>
     <t xml:space="preserve">NAC</t>
@@ -1443,7 +1443,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1506,12 +1506,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -1566,7 +1560,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1619,11 +1613,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1635,7 +1625,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1659,9 +1649,9 @@
   <dimension ref="A1:AH90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G88" activeCellId="0" sqref="G88"/>
+      <selection pane="bottomLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3976,41 +3966,39 @@
         <v>237</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>237</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="K41" s="5" t="n">
-        <v>20674465</v>
+        <v>8996094</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>243</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="M41" s="5"/>
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
@@ -4035,7 +4023,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>245</v>
@@ -4044,33 +4032,35 @@
         <v>14</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="G42" s="5" t="s">
+      <c r="H42" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="I42" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="J42" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="K42" s="5" t="n">
+        <v>20674465</v>
+      </c>
+      <c r="L42" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="K42" s="5" t="n">
-        <v>8996094</v>
-      </c>
-      <c r="L42" s="5" t="s">
+      <c r="M42" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="M42" s="5"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
@@ -4726,7 +4716,7 @@
       <c r="D54" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E54" s="1" t="s">
         <v>307</v>
       </c>
       <c r="F54" s="5" t="s">
@@ -5443,7 +5433,7 @@
       <c r="I68" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J68" s="14" t="s">
+      <c r="J68" s="13" t="s">
         <v>46</v>
       </c>
       <c r="K68" s="9"/>
@@ -5497,7 +5487,7 @@
         <v>384</v>
       </c>
       <c r="I69" s="8"/>
-      <c r="J69" s="14"/>
+      <c r="J69" s="13"/>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
@@ -5549,7 +5539,7 @@
         <v>388</v>
       </c>
       <c r="I70" s="8"/>
-      <c r="J70" s="14"/>
+      <c r="J70" s="13"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
@@ -5601,7 +5591,7 @@
         <v>391</v>
       </c>
       <c r="I71" s="8"/>
-      <c r="J71" s="14"/>
+      <c r="J71" s="13"/>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
@@ -5653,7 +5643,7 @@
         <v>395</v>
       </c>
       <c r="I72" s="8"/>
-      <c r="J72" s="14"/>
+      <c r="J72" s="13"/>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
@@ -5705,7 +5695,7 @@
         <v>400</v>
       </c>
       <c r="I73" s="8"/>
-      <c r="J73" s="14"/>
+      <c r="J73" s="13"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
@@ -5757,7 +5747,7 @@
         <v>404</v>
       </c>
       <c r="I74" s="8"/>
-      <c r="J74" s="14"/>
+      <c r="J74" s="13"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
@@ -5811,7 +5801,7 @@
       <c r="I75" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="J75" s="14" t="s">
+      <c r="J75" s="13" t="s">
         <v>409</v>
       </c>
       <c r="K75" s="9"/>
@@ -5865,7 +5855,7 @@
         <v>413</v>
       </c>
       <c r="I76" s="7"/>
-      <c r="J76" s="14"/>
+      <c r="J76" s="13"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
@@ -5917,9 +5907,9 @@
         <v>417</v>
       </c>
       <c r="I77" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="J77" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="J77" s="13" t="s">
         <v>418</v>
       </c>
       <c r="K77" s="9"/>
@@ -5975,7 +5965,7 @@
       <c r="I78" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="J78" s="14" t="s">
+      <c r="J78" s="13" t="s">
         <v>422</v>
       </c>
       <c r="K78" s="9"/>
@@ -6029,7 +6019,7 @@
         <v>426</v>
       </c>
       <c r="I79" s="8"/>
-      <c r="J79" s="14"/>
+      <c r="J79" s="13"/>
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
@@ -6083,7 +6073,7 @@
       <c r="I80" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="J80" s="14" t="s">
+      <c r="J80" s="13" t="s">
         <v>432</v>
       </c>
       <c r="K80" s="9"/>
@@ -6137,7 +6127,7 @@
         <v>435</v>
       </c>
       <c r="I81" s="8"/>
-      <c r="J81" s="14"/>
+      <c r="J81" s="13"/>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
@@ -6191,7 +6181,7 @@
       <c r="I82" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="J82" s="14" t="s">
+      <c r="J82" s="13" t="s">
         <v>440</v>
       </c>
       <c r="K82" s="9"/>
@@ -6247,7 +6237,7 @@
       <c r="I83" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="J83" s="14" t="s">
+      <c r="J83" s="13" t="s">
         <v>444</v>
       </c>
       <c r="K83" s="9"/>
@@ -6303,7 +6293,7 @@
       <c r="I84" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="J84" s="14" t="s">
+      <c r="J84" s="13" t="s">
         <v>449</v>
       </c>
       <c r="K84" s="9"/>
@@ -6359,7 +6349,7 @@
       <c r="I85" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="J85" s="14" t="s">
+      <c r="J85" s="13" t="s">
         <v>449</v>
       </c>
       <c r="K85" s="9"/>
@@ -6413,7 +6403,7 @@
         <v>453</v>
       </c>
       <c r="I86" s="7"/>
-      <c r="J86" s="14"/>
+      <c r="J86" s="13"/>
       <c r="K86" s="9"/>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
@@ -6465,7 +6455,7 @@
         <v>456</v>
       </c>
       <c r="I87" s="8"/>
-      <c r="J87" s="14"/>
+      <c r="J87" s="13"/>
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
       <c r="M87" s="9"/>
@@ -6519,7 +6509,7 @@
       <c r="I88" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="J88" s="15" t="s">
+      <c r="J88" s="14" t="s">
         <v>461</v>
       </c>
       <c r="K88" s="9"/>
@@ -6575,7 +6565,7 @@
       <c r="I89" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="J89" s="14" t="s">
+      <c r="J89" s="13" t="s">
         <v>467</v>
       </c>
       <c r="K89" s="4"/>
@@ -6604,10 +6594,10 @@
       <c r="AH89" s="4"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E90" s="16" t="s">
+      <c r="E90" s="15" t="s">
         <v>468</v>
       </c>
-      <c r="H90" s="16" t="s">
+      <c r="H90" s="15" t="s">
         <v>469</v>
       </c>
     </row>
@@ -6639,42 +6629,42 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>470</v>
       </c>
     </row>

</xml_diff>